<commit_message>
Updated my part of Gantt Chart
</commit_message>
<xml_diff>
--- a/doc/DeepPurple_Gaant.xlsx
+++ b/doc/DeepPurple_Gaant.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atki7\Documents\CS383\DeepPurple\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\software engineering\DeepPurple\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09A81A9-CED2-4DDC-9DE2-F97820C80398}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C50508-3025-4E71-AC6A-CC5BF92C15E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="67">
   <si>
     <t>hours</t>
   </si>
@@ -226,6 +225,15 @@
   </si>
   <si>
     <t>Testing</t>
+  </si>
+  <si>
+    <t>Designing Characters/ Collect Prefabs</t>
+  </si>
+  <si>
+    <t>Movement Behavior</t>
+  </si>
+  <si>
+    <t>Auxilary Functions</t>
   </si>
 </sst>
 </file>
@@ -506,6 +514,8 @@
     <xf numFmtId="16" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -515,8 +525,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -837,50 +845,50 @@
       <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="3.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="2.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" customWidth="1"/>
+    <col min="5" max="5" width="13.26953125" customWidth="1"/>
+    <col min="6" max="6" width="3.453125" customWidth="1"/>
+    <col min="7" max="7" width="15.26953125" customWidth="1"/>
+    <col min="8" max="8" width="12.26953125" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" customWidth="1"/>
+    <col min="10" max="10" width="2.81640625" customWidth="1"/>
+    <col min="11" max="11" width="13.81640625" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
-    <col min="14" max="14" width="5.42578125" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" customWidth="1"/>
+    <col min="13" max="13" width="14.1796875" customWidth="1"/>
+    <col min="14" max="14" width="5.453125" customWidth="1"/>
+    <col min="15" max="15" width="12.26953125" customWidth="1"/>
+    <col min="16" max="16" width="14.7265625" customWidth="1"/>
+    <col min="17" max="17" width="11.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C2" s="51" t="s">
+    <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="C2" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="53"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="55"/>
       <c r="F2" s="10"/>
-      <c r="G2" s="51" t="s">
+      <c r="G2" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="52"/>
-      <c r="I2" s="53"/>
-      <c r="K2" s="51" t="s">
+      <c r="H2" s="54"/>
+      <c r="I2" s="55"/>
+      <c r="K2" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="52"/>
-      <c r="M2" s="53"/>
-      <c r="O2" s="51" t="s">
+      <c r="L2" s="54"/>
+      <c r="M2" s="55"/>
+      <c r="O2" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="53"/>
-    </row>
-    <row r="3" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P2" s="54"/>
+      <c r="Q2" s="55"/>
+    </row>
+    <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C3" s="11" t="s">
         <v>19</v>
       </c>
@@ -918,7 +926,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B4" s="26" t="s">
         <v>41</v>
       </c>
@@ -969,7 +977,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B5" s="11" t="s">
         <v>37</v>
       </c>
@@ -1020,7 +1028,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B6" s="11" t="s">
         <v>42</v>
       </c>
@@ -1071,7 +1079,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="11" t="s">
         <v>38</v>
       </c>
@@ -1122,7 +1130,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="11" t="s">
         <v>40</v>
       </c>
@@ -1173,7 +1181,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="11" t="s">
         <v>39</v>
       </c>
@@ -1224,7 +1232,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="16" t="s">
         <v>9</v>
       </c>
@@ -1293,19 +1301,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="W30" sqref="W30"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" customWidth="1"/>
+    <col min="6" max="6" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -1328,7 +1336,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>41</v>
       </c>
@@ -1414,7 +1422,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1425,7 +1433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>0</v>
       </c>
@@ -1433,7 +1441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>0</v>
       </c>
@@ -1441,7 +1449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>0</v>
       </c>
@@ -1450,7 +1458,7 @@
       </c>
       <c r="J6" s="50"/>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>0</v>
       </c>
@@ -1458,7 +1466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>0</v>
       </c>
@@ -1466,7 +1474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B9">
         <v>0</v>
       </c>
@@ -1474,7 +1482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B10">
         <f>SUM(B3:B9)</f>
         <v>0</v>
@@ -1483,12 +1491,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -1499,7 +1507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B13">
         <v>0</v>
       </c>
@@ -1507,7 +1515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B14">
         <v>0</v>
       </c>
@@ -1515,7 +1523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B15">
         <v>0</v>
       </c>
@@ -1523,7 +1531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>0</v>
       </c>
@@ -1531,7 +1539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B17">
         <v>0</v>
       </c>
@@ -1539,7 +1547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B18">
         <v>0</v>
       </c>
@@ -1547,7 +1555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B19">
         <v>0</v>
       </c>
@@ -1555,7 +1563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B20">
         <f>SUM(B12:B19)</f>
         <v>0</v>
@@ -1565,12 +1573,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -1580,10 +1588,10 @@
       <c r="C22">
         <v>4</v>
       </c>
-      <c r="E22" s="54"/>
-      <c r="F22" s="55"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E22" s="51"/>
+      <c r="F22" s="52"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -1593,11 +1601,11 @@
       <c r="C23">
         <v>8</v>
       </c>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="54"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="51"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -1607,12 +1615,12 @@
       <c r="C24">
         <v>9</v>
       </c>
-      <c r="H24" s="55"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="54"/>
-      <c r="K24" s="54"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="H24" s="52"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="51"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -1622,14 +1630,14 @@
       <c r="C25">
         <v>12</v>
       </c>
-      <c r="L25" s="54"/>
-      <c r="M25" s="54"/>
-      <c r="N25" s="54"/>
-      <c r="O25" s="54"/>
+      <c r="L25" s="51"/>
+      <c r="M25" s="51"/>
+      <c r="N25" s="51"/>
+      <c r="O25" s="51"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="5"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -1639,7 +1647,7 @@
       <c r="R26" s="5"/>
       <c r="S26" s="5"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>63</v>
       </c>
@@ -1649,55 +1657,75 @@
       <c r="T27" s="5"/>
       <c r="U27" s="5"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="E30" s="51"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>64</v>
+      </c>
       <c r="B31">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>65</v>
+      </c>
       <c r="B32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H32" s="51"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>66</v>
+      </c>
       <c r="B33">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>63</v>
+      </c>
       <c r="B34">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B35">
         <v>0</v>
       </c>
@@ -1705,7 +1733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B36">
         <v>0</v>
       </c>
@@ -1713,12 +1741,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>50</v>
       </c>
@@ -1729,7 +1757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B39">
         <v>0</v>
       </c>
@@ -1737,7 +1765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B40">
         <v>0</v>
       </c>
@@ -1745,7 +1773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B41">
         <v>0</v>
       </c>
@@ -1753,7 +1781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B42">
         <v>0</v>
       </c>
@@ -1761,7 +1789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B43">
         <v>0</v>
       </c>
@@ -1769,7 +1797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B44">
         <v>0</v>
       </c>
@@ -1777,12 +1805,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>51</v>
       </c>
@@ -1793,7 +1821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -1804,7 +1832,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -1815,7 +1843,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>54</v>
       </c>
@@ -1826,7 +1854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>55</v>
       </c>
@@ -1837,7 +1865,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -1848,7 +1876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>57</v>
       </c>
@@ -1859,7 +1887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>58</v>
       </c>
@@ -1870,7 +1898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -1885,6 +1913,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1896,9 +1925,9 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B1" s="8" t="s">
         <v>10</v>
       </c>
@@ -1917,7 +1946,7 @@
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
     </row>
-    <row r="2" spans="1:12" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
         <v>11</v>
       </c>
@@ -1952,7 +1981,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B3" s="8" t="s">
         <v>12</v>
       </c>
@@ -1975,7 +2004,7 @@
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>29</v>
       </c>
@@ -2002,7 +2031,7 @@
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>30</v>
       </c>
@@ -2027,7 +2056,7 @@
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>31</v>
       </c>
@@ -2054,7 +2083,7 @@
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>32</v>
       </c>
@@ -2081,7 +2110,7 @@
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>32</v>
       </c>
@@ -2108,7 +2137,7 @@
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>32</v>
       </c>
@@ -2135,7 +2164,7 @@
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>9</v>
       </c>
@@ -2184,12 +2213,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="7"/>
     </row>
   </sheetData>
@@ -2203,19 +2232,19 @@
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="19" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.7265625" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" customWidth="1"/>
+    <col min="5" max="19" width="3.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="32"/>
       <c r="B1" s="33" t="s">
         <v>24</v>
@@ -2272,7 +2301,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="35" t="s">
         <v>41</v>
       </c>
@@ -2286,7 +2315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="38"/>
       <c r="B3" s="36" t="s">
         <v>34</v>
@@ -2298,7 +2327,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="38"/>
       <c r="B4" s="36" t="s">
         <v>46</v>
@@ -2313,7 +2342,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="38"/>
       <c r="B5" s="36" t="s">
         <v>28</v>
@@ -2327,7 +2356,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="35" t="s">
         <v>37</v>
       </c>
@@ -2341,7 +2370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="38"/>
       <c r="B7" s="36" t="s">
         <v>34</v>
@@ -2353,7 +2382,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="38"/>
       <c r="B8" s="36" t="s">
         <v>47</v>
@@ -2368,7 +2397,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="38"/>
       <c r="B9" s="36" t="s">
         <v>28</v>
@@ -2382,7 +2411,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="35" t="s">
         <v>42</v>
       </c>
@@ -2396,7 +2425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="38"/>
       <c r="B11" s="36" t="s">
         <v>34</v>
@@ -2408,7 +2437,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="38"/>
       <c r="B12" s="36" t="s">
         <v>43</v>
@@ -2423,7 +2452,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="38"/>
       <c r="B13" s="40"/>
       <c r="C13">
@@ -2433,7 +2462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" s="38"/>
       <c r="B14" s="40"/>
       <c r="C14">
@@ -2443,7 +2472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" s="38"/>
       <c r="B15" s="41" t="s">
         <v>28</v>
@@ -2457,7 +2486,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" s="35" t="s">
         <v>38</v>
       </c>
@@ -2471,7 +2500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="38"/>
       <c r="B17" s="36" t="s">
         <v>34</v>
@@ -2483,7 +2512,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="38"/>
       <c r="B18" s="36" t="s">
         <v>45</v>
@@ -2498,7 +2527,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="38"/>
       <c r="B19" s="41" t="s">
         <v>28</v>
@@ -2512,7 +2541,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="35" t="s">
         <v>40</v>
       </c>
@@ -2526,7 +2555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="38"/>
       <c r="B21" s="36" t="s">
         <v>34</v>
@@ -2538,14 +2567,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="38"/>
       <c r="B22" s="36"/>
       <c r="D22" s="37">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="38"/>
       <c r="B23" s="41" t="s">
         <v>28</v>
@@ -2559,7 +2588,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="35" t="s">
         <v>39</v>
       </c>
@@ -2573,7 +2602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="38"/>
       <c r="B25" s="36" t="s">
         <v>34</v>
@@ -2585,7 +2614,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="38"/>
       <c r="B26" s="36" t="s">
         <v>44</v>
@@ -2597,7 +2626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="38"/>
       <c r="B27" s="41" t="s">
         <v>28</v>
@@ -2611,7 +2640,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="42"/>
       <c r="B28" s="43" t="s">
         <v>9</v>
@@ -2625,7 +2654,7 @@
         <v>36.5</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B29" s="31" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Added updated times to master Gantt
</commit_message>
<xml_diff>
--- a/doc/DeepPurple_Gaant.xlsx
+++ b/doc/DeepPurple_Gaant.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\software engineering\DeepPurple\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Documents\GitHub\DeepPurple\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C50508-3025-4E71-AC6A-CC5BF92C15E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1E4A92-1B2B-4BAF-BE96-00CF55C3D715}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="23200" windowHeight="12810" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Management Summary" sheetId="3" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="70">
   <si>
     <t>hours</t>
   </si>
@@ -234,6 +235,15 @@
   </si>
   <si>
     <t>Auxilary Functions</t>
+  </si>
+  <si>
+    <t>Design system</t>
+  </si>
+  <si>
+    <t>Program system</t>
+  </si>
+  <si>
+    <t>Changes after testing</t>
   </si>
 </sst>
 </file>
@@ -458,7 +468,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -515,7 +525,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -866,27 +875,27 @@
   <sheetData>
     <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="55"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="54"/>
       <c r="F2" s="10"/>
-      <c r="G2" s="53" t="s">
+      <c r="G2" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="54"/>
-      <c r="I2" s="55"/>
-      <c r="K2" s="53" t="s">
+      <c r="H2" s="53"/>
+      <c r="I2" s="54"/>
+      <c r="K2" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="54"/>
-      <c r="M2" s="55"/>
-      <c r="O2" s="53" t="s">
+      <c r="L2" s="53"/>
+      <c r="M2" s="54"/>
+      <c r="O2" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="55"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="54"/>
     </row>
     <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C3" s="11" t="s">
@@ -1301,8 +1310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1589,7 +1598,6 @@
         <v>4</v>
       </c>
       <c r="E22" s="51"/>
-      <c r="F22" s="52"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
@@ -1615,7 +1623,6 @@
       <c r="C24">
         <v>9</v>
       </c>
-      <c r="H24" s="52"/>
       <c r="I24" s="51"/>
       <c r="J24" s="51"/>
       <c r="K24" s="51"/>
@@ -1699,7 +1706,7 @@
       </c>
       <c r="H32" s="51"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>66</v>
       </c>
@@ -1712,7 +1719,7 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>63</v>
       </c>
@@ -1725,7 +1732,7 @@
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B35">
         <v>0</v>
       </c>
@@ -1733,7 +1740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B36">
         <v>0</v>
       </c>
@@ -1741,76 +1748,109 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="E38" s="51"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>67</v>
+      </c>
       <c r="B39">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="F39" s="51"/>
+      <c r="G39" s="51"/>
+      <c r="H39" s="51"/>
+      <c r="I39" s="51"/>
+      <c r="J39" s="51"/>
+      <c r="K39" s="51"/>
+      <c r="L39" s="51"/>
+      <c r="M39" s="4"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>68</v>
+      </c>
       <c r="B40">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N40" s="5"/>
+      <c r="O40" s="5"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>54</v>
+      </c>
       <c r="B41">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="P41" s="5"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>63</v>
+      </c>
       <c r="B42">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="Q42" s="5"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>69</v>
+      </c>
       <c r="B43">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="R43" s="5"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>58</v>
+      </c>
       <c r="B44">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="S44" s="5"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>51</v>
       </c>
@@ -1821,7 +1861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -1832,7 +1872,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>53</v>
       </c>

</xml_diff>